<commit_message>
update BOM after assembly
</commit_message>
<xml_diff>
--- a/free2breathe_pcb/BOMrev2.xlsx
+++ b/free2breathe_pcb/BOMrev2.xlsx
@@ -471,7 +471,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +482,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,16 +531,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,6 +565,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -552,21 +636,22 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="91.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -574,15 +659,15 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>44977.6340277778</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -590,7 +675,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -598,7 +683,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -606,7 +691,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -629,7 +714,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -649,7 +734,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -669,10 +754,11 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="n">
         <v>3</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -689,10 +775,11 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="n">
         <v>5</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -709,13 +796,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="5" t="n">
         <v>3</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -732,10 +819,11 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -752,10 +840,11 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="n">
         <v>4</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -772,13 +861,13 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="5" t="n">
         <v>4</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -794,14 +883,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="5" t="n">
         <v>12</v>
       </c>
       <c r="D15" s="0" t="s">
@@ -818,7 +907,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -838,7 +927,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -858,7 +947,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -878,7 +967,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -898,10 +987,11 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5" t="n">
         <v>4</v>
       </c>
       <c r="D20" s="0" t="s">
@@ -918,7 +1008,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -938,13 +1028,13 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="0" t="s">
@@ -958,7 +1048,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -978,7 +1068,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -998,7 +1088,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -1018,10 +1108,11 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="B26" s="4"/>
+      <c r="C26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="0" t="s">
@@ -1038,10 +1129,11 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="B27" s="4"/>
+      <c r="C27" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="0" t="s">
@@ -1058,10 +1150,11 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="B28" s="4"/>
+      <c r="C28" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
@@ -1078,10 +1171,11 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="0" t="s">
@@ -1098,10 +1192,11 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="B30" s="4"/>
+      <c r="C30" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="0" t="s">
@@ -1118,10 +1213,11 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="B31" s="4"/>
+      <c r="C31" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="0" t="s">
@@ -1138,10 +1234,11 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="B32" s="4"/>
+      <c r="C32" s="5" t="n">
         <v>4</v>
       </c>
       <c r="D32" s="0" t="n">
@@ -1158,10 +1255,11 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D33" s="0" t="n">
@@ -1178,7 +1276,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C34" s="0" t="n">
@@ -1198,10 +1296,11 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="0" t="s">
@@ -1218,13 +1317,13 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
@@ -1240,14 +1339,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+    <row r="37" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="5" t="n">
         <v>12</v>
       </c>
       <c r="D37" s="0" t="s">
@@ -1264,13 +1363,13 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D38" s="0" t="s">
@@ -1286,14 +1385,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="5" t="n">
         <v>7</v>
       </c>
       <c r="D39" s="0" t="s">
@@ -1310,13 +1409,13 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="5" t="n">
         <v>4</v>
       </c>
       <c r="D40" s="0" t="n">
@@ -1333,13 +1432,13 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="0" t="s">
@@ -1356,13 +1455,13 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="0" t="s">
@@ -1379,10 +1478,11 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="B43" s="4"/>
+      <c r="C43" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="0" t="s">
@@ -1399,10 +1499,11 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="B44" s="4"/>
+      <c r="C44" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="0" t="n">
@@ -1419,7 +1520,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B45" s="0" t="n">
@@ -1439,13 +1540,13 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D46" s="0" t="s">
@@ -1462,7 +1563,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C47" s="0" t="n">
@@ -1479,7 +1580,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C48" s="0" t="n">
@@ -1496,7 +1597,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C49" s="0" t="n">
@@ -1513,7 +1614,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C50" s="0" t="n">
@@ -1530,7 +1631,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="0" t="n">
@@ -1547,7 +1648,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C52" s="0" t="n">

</xml_diff>